<commit_message>
New Test Cases added - 04/06
</commit_message>
<xml_diff>
--- a/restapi/src/test/java/com/qa/xlsData/TestData.xlsx
+++ b/restapi/src/test/java/com/qa/xlsData/TestData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balaji.balasubramani\eclipse-workspace\restapi\src\test\java\com\qa\xlsData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balaji.balasubramani\git\RestAssured-DT-API\restapi\src\test\java\com\qa\xlsData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11210" windowHeight="2000" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11210" windowHeight="2000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="MeetingEnd" sheetId="2" r:id="rId2"/>
     <sheet name="MeetingPause" sheetId="3" r:id="rId3"/>
     <sheet name="MeetingResume" sheetId="4" r:id="rId4"/>
+    <sheet name="InvokeviaTxt" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="19">
   <si>
     <t>/cvi/dm/api/v1/invoke/intent/json</t>
   </si>
@@ -146,6 +147,19 @@
     ]
   },
   "intent":"MEETING__RESUME"
+}</t>
+  </si>
+  <si>
+    <t>/cvi/dm/api/v1/invoke/text/json?intent=true&amp;skill=true</t>
+  </si>
+  <si>
+    <t>{
+  "text": "starte das toronto meeting"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "text": "starte das Messe meeting"
 }</t>
   </si>
 </sst>
@@ -698,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,4 +779,77 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>